<commit_message>
redirected sending widgets to DynamicPtsSignal
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/TestConfigs.xlsx
+++ b/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/TestConfigs.xlsx
@@ -494,7 +494,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -519,13 +519,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>3</v>
+        <v>44.72666666666667</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -535,7 +535,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>44.73</v>
       </c>
       <c r="E4" t="n">
         <v>20</v>
@@ -550,7 +550,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>44.72666666666667</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started widgets redirect for SinusSignal (still unfinished)
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/TestConfigs.xlsx
+++ b/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/TestConfigs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,7 +494,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -504,7 +504,7 @@
         <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>44.73</v>
       </c>
       <c r="E3" t="n">
         <v>20</v>
@@ -519,37 +519,6 @@
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>44.72666666666667</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>42.55</v>
-      </c>
-      <c r="C4" t="n">
-        <v>20</v>
-      </c>
-      <c r="D4" t="n">
-        <v>44.73</v>
-      </c>
-      <c r="E4" t="n">
-        <v>20</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>20</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
main GUI deleted SignalSendingTab
</commit_message>
<xml_diff>
--- a/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/TestConfigs.xlsx
+++ b/SignalGenerationConfigs/DynamicPointsDensitySignalConfigs/TestConfigs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,14 +494,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>Debug</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>42.55</v>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>63.28</v>
       </c>
       <c r="D3" t="n">
         <v>44.73</v>
@@ -510,7 +510,7 @@
         <v>20</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>2.55</v>
       </c>
       <c r="G3" t="n">
         <v>20</v>
@@ -519,7 +519,38 @@
         <v>1</v>
       </c>
       <c r="I3" t="n">
+        <v>92.72666666666667</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>